<commit_message>
Create POM for joinUs, jobSinglePage, jobApplication,and TCs for Joins E2E
</commit_message>
<xml_diff>
--- a/DataSheet/Test Driven.xlsx
+++ b/DataSheet/Test Driven.xlsx
@@ -4,19 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ContactUs" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="JoinUs" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhKehMECusyUirgHV8dD7Hl8KL6sw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miwCMEqRPJIQKMtuq/OROhiNnFqQA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -55,13 +56,43 @@
   </si>
   <si>
     <t>Mostafaelbehairy@@gmail.com</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>LinkedIn Profile Link</t>
+  </si>
+  <si>
+    <t>Expected Error</t>
+  </si>
+  <si>
+    <t>The field is required.</t>
+  </si>
+  <si>
+    <t>D:\Nucleus\Musala-Website-Automation-master\DataSheet\Mostafa Elbehairy Software Testing - CV.pdf</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/mostafaelbehairy/</t>
+  </si>
+  <si>
+    <t>The e-mail address entered is invalid.</t>
+  </si>
+  <si>
+    <t>Mostafaelbehairy@gmail.com</t>
+  </si>
+  <si>
+    <t>abcdg</t>
+  </si>
+  <si>
+    <t>The telephone number is invalid.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -90,6 +121,37 @@
       <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="3">
@@ -112,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -138,6 +200,37 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -149,6 +242,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -471,4 +568,107 @@
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="5" max="5" width="22.25"/>
+    <col customWidth="1" min="7" max="7" width="36.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1.5399552432E10</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E3"/>
+    <hyperlink r:id="rId2" ref="E4"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>